<commit_message>
Work on duplicating great twitter examples
</commit_message>
<xml_diff>
--- a/Excel_Twitter_Crosscheck.xlsx
+++ b/Excel_Twitter_Crosscheck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{18E41B98-4E93-4DE0-8A51-8F3B8F9C08C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99ABEB3-A492-4AC8-8051-72596B0839E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId4"/>
+    <pivotCache cacheId="8" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="34">
   <si>
     <t>FROM:</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t xml:space="preserve">                    MATCH finds the first value that is exactly equal to lookup_value. The values in the lookup_array argument can be in any order.</t>
+  </si>
+  <si>
+    <t>My Rif:</t>
   </si>
 </sst>
 </file>
@@ -261,7 +264,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -322,6 +325,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -366,7 +375,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8"/>
@@ -376,11 +385,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Comment" xfId="9" xr:uid="{C4DDEBC2-DCD2-4316-AAE7-A5F6C47DBA99}"/>
@@ -737,6 +745,203 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25813301-C87D-49D7-3C06-2C2ED7F1CAEA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5600700" y="670560"/>
+          <a:ext cx="4876800" cy="1615440"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:tabLst>
+              <a:tab pos="182880" algn="l"/>
+            </a:tabLst>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>There are three cases where the frequency function is used:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="182880" indent="-182880">
+            <a:tabLst>
+              <a:tab pos="182880" algn="l"/>
+            </a:tabLst>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:sym typeface="Webdings" panose="05030102010509060703" pitchFamily="18" charset="2"/>
+            </a:rPr>
+            <a:t>	</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>Generate a histogram using (,] ranges, with lower range (-inf,] and top range [,inf)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="182880" indent="-182880">
+            <a:tabLst>
+              <a:tab pos="182880" algn="l"/>
+            </a:tabLst>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:sym typeface="Webdings" panose="05030102010509060703" pitchFamily="18" charset="2"/>
+            </a:rPr>
+            <a:t>	</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>By negating bins and data, generate a histogram using [,) ranges, with lower range [-inf,) and top range [,inf]</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="182880" indent="-182880">
+            <a:tabLst>
+              <a:tab pos="182880" algn="l"/>
+            </a:tabLst>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:sym typeface="Webdings" panose="05030102010509060703" pitchFamily="18" charset="2"/>
+            </a:rPr>
+            <a:t>	</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>If you set the data and bin ranges equal, you get a frequency count of the number of times every item occurs (0s after first occurrence). </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>335280</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1181100</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Callout: Line with No Border 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D3372DB-06DA-CE16-6DA0-D731154B9F23}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6012180" y="5867400"/>
+          <a:ext cx="2606040" cy="289560"/>
+        </a:xfrm>
+        <a:prstGeom prst="callout1">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 18750"/>
+            <a:gd name="adj2" fmla="val -8333"/>
+            <a:gd name="adj3" fmla="val -21711"/>
+            <a:gd name="adj4" fmla="val -21898"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Always have one extra cell</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -868,7 +1073,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B17:F28" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -1160,10 +1365,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="B4:H46"/>
+  <dimension ref="B3:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1172,10 +1377,18 @@
     <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.77734375" customWidth="1"/>
+    <col min="12" max="12" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <f>ROWS(C5:C26)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>21</v>
       </c>
@@ -1186,25 +1399,25 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="10">
         <v>225642485</v>
       </c>
       <c r="D5" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="9">
         <v>7843</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="11">
         <v>21548</v>
       </c>
       <c r="D6" t="s">
@@ -1214,21 +1427,21 @@
         <v>452</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="10">
         <v>225642485</v>
       </c>
       <c r="D7" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="9">
         <v>9656</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>24</v>
       </c>
@@ -1238,25 +1451,25 @@
       <c r="D8" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="9">
         <v>3547</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="11">
         <v>21548</v>
       </c>
       <c r="D10" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="9">
         <v>6086</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>27</v>
       </c>
@@ -1266,11 +1479,11 @@
       <c r="D11" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="9">
         <v>3452</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>28</v>
       </c>
@@ -1280,11 +1493,11 @@
       <c r="D12" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="9">
         <v>1238</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>29</v>
       </c>
@@ -1294,25 +1507,25 @@
       <c r="D13" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="9">
         <v>7625</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="11">
         <v>21548</v>
       </c>
       <c r="D15" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="9">
         <v>5380</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>27</v>
       </c>
@@ -1322,22 +1535,49 @@
       <c r="D16" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="9">
         <v>4046</v>
       </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H17" s="11" cm="1">
-        <f t="array" ref="H17:H34">FREQUENCY(C5:C26,C5:C26)</f>
+      <c r="H16" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="H18" s="12" cm="1">
+        <f t="array" ref="H18:H35">FREQUENCY(C5:C26,C5:C26)</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H18" s="12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="12" cm="1">
+        <f t="array" ref="I18:I34">_xlfn._xlws.FILTER(C5:C26,LEN(C5:C26)&gt;0)</f>
+        <v>225642485</v>
+      </c>
+      <c r="J18" s="12" cm="1">
+        <f t="array" ref="J18:J21">_xlfn.UNIQUE(_xlfn._xlws.FILTER(C5:C26,LEN(C5:C26)&lt;&gt;0))</f>
+        <v>225642485</v>
+      </c>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12" cm="1">
+        <f t="array" ref="L18:M21">_xlfn.LET(_xlpm.x,_xlfn._xlws.FILTER(C5:C26,LEN(C5:C26)&gt;0),_xlpm.y,_xlfn.HSTACK(_xlpm.x,FREQUENCY(_xlpm.x,_xlpm.x)),_xlfn._xlws.FILTER(_xlpm.y,_xlfn.TAKE(_xlpm.y,,-1)))</f>
+        <v>225642485</v>
+      </c>
+      <c r="M18" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>28</v>
       </c>
@@ -1347,18 +1587,31 @@
       <c r="D19" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="9">
         <v>7594</v>
       </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H19" s="12">
+        <v>5</v>
+      </c>
+      <c r="I19" s="12">
+        <v>21548</v>
+      </c>
+      <c r="J19" s="12">
+        <v>21548</v>
+      </c>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12">
+        <v>21548</v>
+      </c>
+      <c r="M19" s="12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C20" s="10">
         <v>225642485</v>
       </c>
       <c r="D20" t="s">
@@ -1367,67 +1620,114 @@
       <c r="E20">
         <v>991</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="12">
+        <v>0</v>
+      </c>
+      <c r="I20" s="12">
+        <v>225642485</v>
+      </c>
+      <c r="J20" s="12">
+        <v>35486548798</v>
+      </c>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12">
+        <v>35486548798</v>
+      </c>
+      <c r="M20" s="12">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C21" s="10">
         <v>225642485</v>
       </c>
       <c r="D21" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E21" s="9">
         <v>4441</v>
       </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H21" s="12">
+        <v>6</v>
+      </c>
+      <c r="I21" s="12">
+        <v>35486548798</v>
+      </c>
+      <c r="J21" s="12">
+        <v>332699</v>
+      </c>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12">
+        <v>332699</v>
+      </c>
+      <c r="M21" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="13">
+      <c r="C22" s="11">
         <v>21548</v>
       </c>
       <c r="D22" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E22" s="9">
         <v>1555</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="12">
+        <v>0</v>
+      </c>
+      <c r="I22" s="12">
+        <v>21548</v>
+      </c>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="H23" s="12">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I23" s="12">
+        <v>332699</v>
+      </c>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="13">
+      <c r="C24" s="11">
         <v>21548</v>
       </c>
       <c r="D24" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E24" s="9">
         <v>8868</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="12">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I24" s="12">
+        <v>35486548798</v>
+      </c>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>29</v>
       </c>
@@ -1437,14 +1737,26 @@
       <c r="D25" t="s">
         <v>25</v>
       </c>
-      <c r="E25" s="10">
+      <c r="E25" s="9">
         <v>6475</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="12">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I25" s="12">
+        <v>35486548798</v>
+      </c>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12" cm="1">
+        <f t="array" ref="L25:M28">_xlfn.LAMBDA(_xlpm.x,_xlfn.LET(_xlpm.x,_xlfn._xlws.FILTER(_xlpm.x,LEN(_xlpm.x)&gt;0),_xlpm.y,_xlfn.HSTACK(_xlpm.x,FREQUENCY(_xlpm.x,_xlpm.x)),_xlfn._xlws.FILTER(_xlpm.y,_xlfn.TAKE(_xlpm.y,,-1))))(C5:C26)</f>
+        <v>225642485</v>
+      </c>
+      <c r="M25" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>28</v>
       </c>
@@ -1454,111 +1766,214 @@
       <c r="D26" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="10">
+      <c r="E26" s="9">
         <v>7430</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="12">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H27">
+      <c r="I26" s="12">
+        <v>21548</v>
+      </c>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12">
+        <v>21548</v>
+      </c>
+      <c r="M26" s="12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="H27" s="12">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H28">
+      <c r="I27" s="12">
+        <v>35486548798</v>
+      </c>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12">
+        <v>35486548798</v>
+      </c>
+      <c r="M27" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="H28" s="12">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I28" s="12">
+        <v>35486548798</v>
+      </c>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12">
+        <v>332699</v>
+      </c>
+      <c r="M28" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29">
         <f>MODE(C5:C26)</f>
         <v>35486548798</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="12">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H30">
+      <c r="I29" s="12">
+        <v>225642485</v>
+      </c>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="H30" s="12">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I30" s="12">
+        <v>225642485</v>
+      </c>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" cm="1">
         <f t="array" ref="B31">MODE(IF(C5:C26&lt;&gt;"",IF(C5:C26&lt;&gt;MODE(C5:C26),C5:C26)))</f>
         <v>21548</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="12">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H32">
+      <c r="I31" s="12">
+        <v>21548</v>
+      </c>
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="12"/>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="H32" s="12">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I32" s="12">
+        <v>21548</v>
+      </c>
+      <c r="J32" s="12"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="12"/>
+      <c r="M32" s="12"/>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33">
         <f>INDEX(C5:C26,MATCH(LARGE(FREQUENCY(C5:C26,C5:C26),3),FREQUENCY(C5:C26,C5:C26),0))</f>
         <v>225642485</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="12">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H34">
+      <c r="I33" s="12">
+        <v>35486548798</v>
+      </c>
+      <c r="J33" s="12"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="12"/>
+      <c r="M33" s="12"/>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="H34" s="12">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I34" s="12">
+        <v>332699</v>
+      </c>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="12"/>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="H35" s="12">
+        <v>0</v>
+      </c>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="12"/>
+      <c r="M35" s="12"/>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="12"/>
+      <c r="M36" s="12"/>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="12"/>
+      <c r="K37" s="12"/>
+      <c r="L37" s="12"/>
+      <c r="M37" s="12"/>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="12"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="12"/>
+      <c r="M38" s="12"/>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C42">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
         <v>32</v>
       </c>
@@ -1607,7 +2022,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>13-Apr-2024</v>
+        <v>14-Apr-2024</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -1743,19 +2158,15 @@
       <c r="B19" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>1</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20">
         <v>1</v>
       </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9">
+      <c r="F20">
         <v>1</v>
       </c>
     </row>
@@ -1763,11 +2174,10 @@
       <c r="C21">
         <v>2</v>
       </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9">
+      <c r="E21">
         <v>2</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21">
         <v>2</v>
       </c>
     </row>
@@ -1775,19 +2185,15 @@
       <c r="B22" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>1</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23">
         <v>3</v>
       </c>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9">
+      <c r="F23">
         <v>3</v>
       </c>
     </row>
@@ -1795,11 +2201,10 @@
       <c r="C24">
         <v>2</v>
       </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9">
+      <c r="E24">
         <v>4</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F24">
         <v>4</v>
       </c>
     </row>
@@ -1807,19 +2212,15 @@
       <c r="B25" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D26">
         <v>5</v>
       </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9">
+      <c r="F26">
         <v>5</v>
       </c>
     </row>
@@ -1827,11 +2228,10 @@
       <c r="C27">
         <v>2</v>
       </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9">
+      <c r="E27">
         <v>6</v>
       </c>
-      <c r="F27" s="9">
+      <c r="F27">
         <v>6</v>
       </c>
     </row>
@@ -1839,13 +2239,13 @@
       <c r="B28" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D28">
         <v>9</v>
       </c>
-      <c r="E28" s="9">
+      <c r="E28">
         <v>12</v>
       </c>
-      <c r="F28" s="9">
+      <c r="F28">
         <v>21</v>
       </c>
     </row>
@@ -1918,7 +2318,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>13-Apr-2024</v>
+        <v>14-Apr-2024</v>
       </c>
       <c r="C3" s="2"/>
     </row>

</xml_diff>

<commit_message>
Searching for special cells
</commit_message>
<xml_diff>
--- a/Excel_Twitter_Crosscheck.xlsx
+++ b/Excel_Twitter_Crosscheck.xlsx
@@ -8,21 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99ABEB3-A492-4AC8-8051-72596B0839E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9752F252-BD07-4217-8534-8C38BEB4A3EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
-    <sheet name="Report" sheetId="1" r:id="rId1"/>
-    <sheet name="Formats" sheetId="2" r:id="rId2"/>
-    <sheet name="Lists" sheetId="3" r:id="rId3"/>
+    <sheet name="Frequency" sheetId="1" r:id="rId1"/>
+    <sheet name="SpecialCellSearch" sheetId="4" r:id="rId2"/>
+    <sheet name="Formats" sheetId="2" r:id="rId3"/>
+    <sheet name="Lists" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="_nList">SpecialCellSearch!$B$8:$B$27</definedName>
     <definedName name="HD_Date">_xlfn.LET(_xlpm.dt, TODAY(),      _xlpm.y,  YEAR(_xlpm.dt),      _xlpm.m,  MONTH(_xlpm.dt),      _xlpm.d,  DAY(_xlpm.dt),      TEXT(DATE(_xlpm.y,_xlpm.m,_xlpm.d),"dd-mmm-yyyy")     )</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId4"/>
+    <pivotCache cacheId="9" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,6 +37,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -64,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="47">
   <si>
     <t>FROM:</t>
   </si>
@@ -166,6 +170,45 @@
   </si>
   <si>
     <t>My Rif:</t>
+  </si>
+  <si>
+    <t>Finding Spell Numbers</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>Excel</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>Spreadsheet</t>
+  </si>
+  <si>
+    <t>List</t>
+  </si>
+  <si>
+    <t>Last Number</t>
+  </si>
+  <si>
+    <t>Cell Address, Absolute</t>
+  </si>
+  <si>
+    <t>Actually, it is is relative within list</t>
+  </si>
+  <si>
+    <t>Cell Address, Relative</t>
+  </si>
+  <si>
+    <t>Last Text</t>
+  </si>
+  <si>
+    <t>Cell address, absolute</t>
+  </si>
+  <si>
+    <t>Cell address, relative</t>
   </si>
 </sst>
 </file>
@@ -375,7 +418,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8"/>
@@ -389,6 +432,10 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="15" fontId="6" fillId="4" borderId="0" xfId="8" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="9"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Comment" xfId="9" xr:uid="{C4DDEBC2-DCD2-4316-AAE7-A5F6C47DBA99}"/>
@@ -949,6 +996,72 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Image">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C9E9FF5-C939-00F6-20D6-3585EA0A6F41}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9144000" y="502920"/>
+          <a:ext cx="9166860" cy="5318760"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
       <xdr:row>1</xdr:row>
@@ -1073,7 +1186,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B17:F28" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -1367,8 +1480,8 @@
   </sheetPr>
   <dimension ref="B3:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1985,6 +2098,272 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF67CF35-5498-4338-9495-540D68BAE206}">
+  <dimension ref="A1:M27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" customWidth="1"/>
+    <col min="4" max="4" width="27" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="13">
+        <v>45396</v>
+      </c>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8">
+        <f>LOOKUP(9.9999999999999E+307,_nList)</f>
+        <v>-4</v>
+      </c>
+      <c r="F8" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(E8)</f>
+        <v>=LOOKUP(9.9999999999999E+307,_nList)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" t="str">
+        <f>ADDRESS(MATCH(9.999999999E+307,_nList),1)</f>
+        <v>$A$20</v>
+      </c>
+      <c r="F9" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(E9)</f>
+        <v>=ADDRESS(MATCH(9.999999999E+307,_nList),1)</v>
+      </c>
+      <c r="M9" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" t="str">
+        <f>SUBSTITUTE(ADDRESS(MATCH(9.999999999E+307,_nList),1),"$","")</f>
+        <v>A20</v>
+      </c>
+      <c r="F10" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(E10)</f>
+        <v>=SUBSTITUTE(ADDRESS(MATCH(9.999999999E+307,_nList),1),"$","")</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" t="str">
+        <f>INDEX(_nList,MATCH("*",_nList,-1))</f>
+        <v>Spreadsheet</v>
+      </c>
+      <c r="F11" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(E11)</f>
+        <v>=INDEX(_nList,MATCH("*",_nList,-1))</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" t="str">
+        <f>ADDRESS(MATCH(REPT("z",255),_nList),1,1)</f>
+        <v>$A$15</v>
+      </c>
+      <c r="F12" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(E12)</f>
+        <v>=ADDRESS(MATCH(REPT("z",255),_nList),1,1)</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" t="str">
+        <f>SUBSTITUTE(ADDRESS(MATCH(REPT("z",255),_nList),1,1),"$","")</f>
+        <v>A15</v>
+      </c>
+      <c r="F13" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(E13)</f>
+        <v>=SUBSTITUTE(ADDRESS(MATCH(REPT("z",255),_nList),1,1),"$","")</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>11</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>13</v>
+      </c>
+      <c r="B20">
+        <v>-32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>14</v>
+      </c>
+      <c r="B21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>15</v>
+      </c>
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>17</v>
+      </c>
+      <c r="B24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>20</v>
+      </c>
+      <c r="B27">
+        <v>-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{912E8867-A2D1-43A4-9ACC-7AB2760F7CD8}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
@@ -2283,7 +2662,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E13436D-CE0C-4639-B951-C1B98556791F}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>

</xml_diff>